<commit_message>
Reduced log file size for Mode A2 log
8/13/2025: Several versions of the message log for running history questions with the -a2-log version of the LLM system were created and tested. The one ending in _trimmed-2-csv seemed to get the same correct answers as the next larger one, but it is significantly smaller. A reference to that file is being left in the .json file.
Message-Logs.xslx gives some comparisons of these various files.
</commit_message>
<xml_diff>
--- a/src/pysoarlib/connectors/language_model/templates/examples/ship/Message-Logs.xlsx
+++ b/src/pysoarlib/connectors/language_model/templates/examples/ship/Message-Logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\pysoarlib\src\pysoarlib\connectors\language_model\templates\examples\ship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F622A19D-757F-42D8-A596-678EEE2FF936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E3583E-F899-4FFD-9320-E0959FB42574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-5520" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>File Name</t>
   </si>
@@ -110,6 +110,18 @@
   </si>
   <si>
     <t>_reversed.csv</t>
+  </si>
+  <si>
+    <t>ship-question-mode-a2-200-log csv2</t>
+  </si>
+  <si>
+    <t>_trimmed-2.csv</t>
+  </si>
+  <si>
+    <t>message-log-200_trimmed-2.csv</t>
+  </si>
+  <si>
+    <t>Removed unneeded columns, port-id-&gt;next-port</t>
   </si>
 </sst>
 </file>
@@ -436,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -548,6 +560,20 @@
         <v>14</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="1">
+        <v>403</v>
+      </c>
+      <c r="C8" s="2">
+        <v>47122</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="92" orientation="portrait" r:id="rId1"/>
@@ -556,10 +582,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62C0889E-8AFC-477D-8F2C-F27A6A77A2BD}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -655,6 +681,23 @@
         <v>2</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="1">
+        <v>28.549600000000002</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2.8549600000000002</v>
+      </c>
+      <c r="E6" s="1">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="97" orientation="portrait" r:id="rId1"/>

</xml_diff>